<commit_message>
Adjust housekeeping power supplies to remove output filter network
</commit_message>
<xml_diff>
--- a/DC-DC MC3x063A Step-Down Calcs.xlsx
+++ b/DC-DC MC3x063A Step-Down Calcs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaitl\OneDrive\Documents\IEEE RAS\robomaster_hardware\SupercapManager\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tachi\Documents\robomaster_hardware\SupercapManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B952538B-15A4-4641-A1B3-8C73B2261098}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84D40D0A-F38B-493B-8ABB-FA7AECA5F344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{BA15FB53-F390-45F1-BA65-739C49313D22}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{BA15FB53-F390-45F1-BA65-739C49313D22}"/>
   </bookViews>
   <sheets>
     <sheet name="DC-DC MC3x063A Step-Down Calcs" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
   <si>
     <t>Typical</t>
   </si>
@@ -582,6 +582,15 @@
       </rPr>
       <t xml:space="preserve"> to minimize ripple?</t>
     </r>
+  </si>
+  <si>
+    <t>Lmin</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>Minimum inductance</t>
   </si>
 </sst>
 </file>
@@ -591,7 +600,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -744,7 +753,7 @@
       <xdr:col>15</xdr:col>
       <xdr:colOff>44782</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>48062</xdr:rowOff>
+      <xdr:rowOff>21356</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1101,23 +1110,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9206E603-A3C9-44DE-A224-17BD2D7050D1}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="107" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="107" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="6.1796875" customWidth="1"/>
-    <col min="2" max="2" width="8.1796875" customWidth="1"/>
-    <col min="3" max="3" width="5.1796875" customWidth="1"/>
-    <col min="4" max="4" width="6.54296875" customWidth="1"/>
-    <col min="5" max="5" width="37.453125" customWidth="1"/>
-    <col min="6" max="6" width="4.7265625" customWidth="1"/>
+    <col min="1" max="1" width="6.125" customWidth="1"/>
+    <col min="2" max="2" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.125" customWidth="1"/>
+    <col min="4" max="4" width="6.5" customWidth="1"/>
+    <col min="5" max="5" width="37.5" customWidth="1"/>
+    <col min="6" max="6" width="4.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1138,7 +1147,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" ht="18.75">
       <c r="A2" s="10" t="s">
         <v>12</v>
       </c>
@@ -1158,7 +1167,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" ht="18.75">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1178,7 +1187,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" ht="16.5">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
@@ -1194,7 +1203,7 @@
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" ht="16.5">
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
@@ -1210,7 +1219,7 @@
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" ht="18.75">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1225,7 +1234,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:7" ht="19.5" thickBot="1">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -1239,7 +1248,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="17" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" ht="19.5" thickTop="1">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1252,7 +1261,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:7" ht="19.5" thickBot="1">
       <c r="A9" s="7" t="s">
         <v>10</v>
       </c>
@@ -1266,7 +1275,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="17" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" ht="19.5" thickTop="1">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1281,7 +1290,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" ht="18.75">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1297,7 +1306,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:7" ht="19.5" thickBot="1">
       <c r="A12" s="7" t="s">
         <v>8</v>
       </c>
@@ -1313,7 +1322,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="17" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" ht="17.25" thickTop="1">
       <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
@@ -1329,7 +1338,7 @@
       </c>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:7" ht="19.5" thickBot="1">
       <c r="A14" s="7" t="s">
         <v>16</v>
       </c>
@@ -1345,7 +1354,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="17" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" ht="17.25" thickTop="1">
       <c r="A15" s="1" t="s">
         <v>40</v>
       </c>
@@ -1361,36 +1370,48 @@
       </c>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
+    <row r="16" spans="1:7" ht="19.5" thickBot="1">
+      <c r="A16" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="7">
         <f>((B14)*(B11+B12))/(8*B15)</f>
         <v>6.3307883522727279E-3</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" t="s">
+      <c r="C16" s="8"/>
+      <c r="D16" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B17" s="2"/>
+    <row r="17" spans="1:5" ht="15.75" thickTop="1">
+      <c r="A17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="9">
+        <f>(B4-B3-B5)/B14*B11</f>
+        <v>7.9312499999999999E-4</v>
+      </c>
       <c r="C17" s="4"/>
-    </row>
-    <row r="18" spans="1:3" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="4"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="B19" s="2"/>
       <c r="C19" s="4"/>
+    </row>
+    <row r="20" spans="1:5" ht="18.75">
+      <c r="A20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -1405,23 +1426,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="430f76a6-8bad-4da0-9463-45cb17384a94" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100148FEC1369C58D489D1A1EE5D38CC7E2" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="34d7f135eea8b250643856f19a8859c5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="430f76a6-8bad-4da0-9463-45cb17384a94" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="98165b78c0e22eecc28731fb4b51a4da" ns3:_="">
     <xsd:import namespace="430f76a6-8bad-4da0-9463-45cb17384a94"/>
@@ -1603,31 +1607,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9D903D87-60BF-4E03-956B-7F9A5E117B49}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="430f76a6-8bad-4da0-9463-45cb17384a94"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7B8F67C-092F-4C9C-8E71-784893529E69}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="430f76a6-8bad-4da0-9463-45cb17384a94" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7B58015-8DAB-47BD-AA9E-0D418F8B5C40}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1643,4 +1640,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7B8F67C-092F-4C9C-8E71-784893529E69}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9D903D87-60BF-4E03-956B-7F9A5E117B49}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="430f76a6-8bad-4da0-9463-45cb17384a94"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>